<commit_message>
added first day attendance
</commit_message>
<xml_diff>
--- a/attendance-sheet.xlsx
+++ b/attendance-sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Documents/trainings/general/react/react-itc-may-14-31-2018/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69DF25AF-6942-924C-98D5-25551051501F}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{293C51E9-088A-0248-A7ED-9E7FF88FD67D}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14660" xr2:uid="{CBB9C8E6-5B3B-8049-96F8-54CD5DF45308}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
   <si>
     <t>PS ID</t>
   </si>
@@ -172,6 +172,12 @@
   </si>
   <si>
     <t>22-May-18</t>
+  </si>
+  <si>
+    <t>Nitin Ratti</t>
+  </si>
+  <si>
+    <t>Shefali</t>
   </si>
 </sst>
 </file>
@@ -224,7 +230,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -248,6 +254,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -374,7 +392,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -392,14 +410,8 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="15" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="15" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="15" fontId="1" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -412,6 +424,15 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="1" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
@@ -419,48 +440,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="13">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="27" formatCode="dd/mm/yy\ h:mm"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -817,13 +796,6 @@
       </border>
     </dxf>
     <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -863,6 +835,55 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="27" formatCode="dd/mm/yy\ h:mm"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -877,7 +898,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7C6CFE7A-9743-8149-9A78-124B6B70875A}" name="Attendance_Sheet" displayName="Attendance_Sheet" ref="B1:I21" totalsRowShown="0" headerRowDxfId="0" dataDxfId="12" headerRowBorderDxfId="10" tableBorderDxfId="11" totalsRowBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7C6CFE7A-9743-8149-9A78-124B6B70875A}" name="Attendance_Sheet" displayName="Attendance_Sheet" ref="B1:I21" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11" tableBorderDxfId="9" totalsRowBorderDxfId="8">
   <autoFilter ref="B1:I21" xr:uid="{DE7A6E70-F58E-C249-9467-AC9E70F30214}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -889,14 +910,14 @@
     <filterColumn colId="7" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{11970068-BC53-734C-9B64-0C4F81F9A0A8}" name="PS ID" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{86FF5815-B1B0-3640-A190-436A829B7AA3}" name="Email ID" dataDxfId="7" dataCellStyle="Hyperlink"/>
-    <tableColumn id="4" xr3:uid="{E6EFBAEC-EB31-BB43-9BAF-7880E691B687}" name="14-May-18" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{A745971A-1BB0-154A-BCF6-8E8BFAA8A941}" name="16-May-18" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{D381E8B0-CBB1-9D4D-B337-C7D735049830}" name="17-May-18" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{68643B6E-BD17-CE45-B4A8-F32015BC9A1E}" name="19-May-18" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{F1BC98DC-1CF6-DC47-AE71-C55FF6802BA3}" name="20-May-18" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{C7A5AEB7-5456-9D46-939E-9D0DAA9A2AFB}" name="22-May-18" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{11970068-BC53-734C-9B64-0C4F81F9A0A8}" name="PS ID" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{86FF5815-B1B0-3640-A190-436A829B7AA3}" name="Email ID" dataDxfId="6" dataCellStyle="Hyperlink"/>
+    <tableColumn id="4" xr3:uid="{E6EFBAEC-EB31-BB43-9BAF-7880E691B687}" name="14-May-18" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{A745971A-1BB0-154A-BCF6-8E8BFAA8A941}" name="16-May-18" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{D381E8B0-CBB1-9D4D-B337-C7D735049830}" name="17-May-18" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{68643B6E-BD17-CE45-B4A8-F32015BC9A1E}" name="19-May-18" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{F1BC98DC-1CF6-DC47-AE71-C55FF6802BA3}" name="20-May-18" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{C7A5AEB7-5456-9D46-939E-9D0DAA9A2AFB}" name="22-May-18" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark7" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
 </table>
@@ -1203,7 +1224,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A17" sqref="A17"/>
+      <selection pane="topRight" activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1218,7 +1239,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="16" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -1227,22 +1248,22 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="H1" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="I1" s="19" t="s">
+      <c r="I1" s="13" t="s">
         <v>48</v>
       </c>
       <c r="J1" s="1"/>
@@ -1260,22 +1281,22 @@
       <c r="A2" s="5"/>
       <c r="B2" s="4"/>
       <c r="C2" s="5"/>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="H2" s="20" t="s">
+      <c r="H2" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="I2" s="21" t="s">
+      <c r="I2" s="15" t="s">
         <v>41</v>
       </c>
       <c r="J2" s="1"/>
@@ -1299,12 +1320,12 @@
       <c r="C3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="11"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="20"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
@@ -1316,12 +1337,12 @@
       <c r="C4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="12"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="21"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
@@ -1333,12 +1354,12 @@
       <c r="C5" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="12"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="21"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
@@ -1350,12 +1371,12 @@
       <c r="C6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="12"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="21"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
@@ -1367,12 +1388,12 @@
       <c r="C7" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="12"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="21"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
@@ -1384,12 +1405,12 @@
       <c r="C8" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="12"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="21"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
@@ -1401,12 +1422,12 @@
       <c r="C9" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="12"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="21"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
@@ -1418,12 +1439,12 @@
       <c r="C10" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="12"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="21"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
@@ -1435,12 +1456,12 @@
       <c r="C11" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="12"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="21"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
@@ -1452,12 +1473,12 @@
       <c r="C12" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="12"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="21"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
@@ -1469,12 +1490,12 @@
       <c r="C13" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="12"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="21"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
@@ -1486,12 +1507,12 @@
       <c r="C14" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="12"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="21"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
@@ -1503,12 +1524,12 @@
       <c r="C15" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="12"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="21"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
@@ -1520,12 +1541,12 @@
       <c r="C16" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="12"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="21"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
@@ -1537,12 +1558,12 @@
       <c r="C17" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="12"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="21"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
@@ -1554,12 +1575,12 @@
       <c r="C18" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="12"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="21"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
@@ -1571,12 +1592,12 @@
       <c r="C19" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="12"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="21"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
@@ -1588,32 +1609,58 @@
       <c r="C20" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="12"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="21"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="13">
+      <c r="B21" s="9">
         <v>13266</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C21" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
-      <c r="I21" s="16"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="22"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="23"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22" s="9"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="22"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" s="7"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="22"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="G27" s="17"/>
+      <c r="G27" s="11"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
before start of session on may 22
</commit_message>
<xml_diff>
--- a/attendance-sheet.xlsx
+++ b/attendance-sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Documents/trainings/general/react/react-itc-may-14-31-2018/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9FF8EDE-C771-8248-851B-76CD7C56C29F}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96D36447-5EDD-E448-9D74-3D5C325BC09E}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14660" xr2:uid="{CBB9C8E6-5B3B-8049-96F8-54CD5DF45308}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="53">
   <si>
     <t>PS ID</t>
   </si>
@@ -177,7 +177,13 @@
     <t>Nitin Ratti</t>
   </si>
   <si>
-    <t>Shefali</t>
+    <t>Shefali Garg</t>
+  </si>
+  <si>
+    <t>shefali.g@itcinfotech.com</t>
+  </si>
+  <si>
+    <t>Veereshwari Sajjanar</t>
   </si>
 </sst>
 </file>
@@ -286,7 +292,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -410,6 +416,17 @@
         <color indexed="64"/>
       </left>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -420,7 +437,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -469,6 +486,7 @@
     <xf numFmtId="0" fontId="6" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
@@ -934,8 +952,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7C6CFE7A-9743-8149-9A78-124B6B70875A}" name="Attendance_Sheet" displayName="Attendance_Sheet" ref="B1:I21" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11" tableBorderDxfId="9" totalsRowBorderDxfId="8">
-  <autoFilter ref="B1:I21" xr:uid="{DE7A6E70-F58E-C249-9467-AC9E70F30214}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7C6CFE7A-9743-8149-9A78-124B6B70875A}" name="Attendance_Sheet" displayName="Attendance_Sheet" ref="B1:I23" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11" tableBorderDxfId="9" totalsRowBorderDxfId="8">
+  <autoFilter ref="B1:I23" xr:uid="{DE7A6E70-F58E-C249-9467-AC9E70F30214}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -1256,11 +1274,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8890E798-F38F-8643-943F-E0FFFE37A055}">
-  <dimension ref="A1:S27"/>
+  <dimension ref="A1:S26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A4" sqref="A4"/>
+      <selection pane="topRight" activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1473,9 +1491,9 @@
         <v>10</v>
       </c>
       <c r="D6" s="17"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
       <c r="H6" s="18"/>
       <c r="I6" s="21"/>
       <c r="J6" s="21"/>
@@ -1603,10 +1621,10 @@
         <v>20</v>
       </c>
       <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
       <c r="I11" s="21"/>
       <c r="J11" s="21"/>
       <c r="K11" s="21"/>
@@ -1776,65 +1794,61 @@
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" s="6">
-        <v>28126</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D18" s="17"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="18"/>
-      <c r="I18" s="21"/>
-      <c r="J18" s="21"/>
-      <c r="K18" s="21"/>
-      <c r="L18" s="21"/>
-      <c r="M18" s="29"/>
-      <c r="N18" s="29"/>
-      <c r="O18" s="21"/>
-      <c r="P18" s="21"/>
-      <c r="Q18" s="21"/>
-      <c r="R18" s="21"/>
+        <v>49</v>
+      </c>
+      <c r="B18" s="9"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
+      <c r="K18" s="22"/>
+      <c r="L18" s="22"/>
+      <c r="M18" s="31"/>
+      <c r="N18" s="31"/>
+      <c r="O18" s="22"/>
+      <c r="P18" s="22"/>
+      <c r="Q18" s="22"/>
+      <c r="R18" s="22"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B19" s="6">
-        <v>4461</v>
+        <v>50</v>
+      </c>
+      <c r="B19" s="7">
+        <v>24401</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D19" s="17"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="21"/>
-      <c r="J19" s="21"/>
-      <c r="K19" s="21"/>
-      <c r="L19" s="21"/>
-      <c r="M19" s="29"/>
-      <c r="N19" s="29"/>
-      <c r="O19" s="21"/>
-      <c r="P19" s="21"/>
-      <c r="Q19" s="21"/>
-      <c r="R19" s="21"/>
+        <v>51</v>
+      </c>
+      <c r="D19" s="18"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="22"/>
+      <c r="J19" s="22"/>
+      <c r="K19" s="22"/>
+      <c r="L19" s="22"/>
+      <c r="M19" s="18"/>
+      <c r="N19" s="18"/>
+      <c r="O19" s="22"/>
+      <c r="P19" s="22"/>
+      <c r="Q19" s="22"/>
+      <c r="R19" s="22"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B20" s="6">
-        <v>9133</v>
+        <v>28126</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D20" s="17"/>
       <c r="E20" s="18"/>
@@ -1845,8 +1859,8 @@
       <c r="J20" s="21"/>
       <c r="K20" s="21"/>
       <c r="L20" s="21"/>
-      <c r="M20" s="29"/>
-      <c r="N20" s="29"/>
+      <c r="M20" s="18"/>
+      <c r="N20" s="18"/>
       <c r="O20" s="21"/>
       <c r="P20" s="21"/>
       <c r="Q20" s="21"/>
@@ -1854,76 +1868,106 @@
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B21" s="9">
-        <v>13266</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="D21" s="24"/>
-      <c r="E21" s="22"/>
-      <c r="F21" s="22"/>
-      <c r="G21" s="22"/>
-      <c r="H21" s="22"/>
-      <c r="I21" s="23"/>
-      <c r="J21" s="23"/>
-      <c r="K21" s="23"/>
-      <c r="L21" s="23"/>
-      <c r="M21" s="30"/>
-      <c r="N21" s="30"/>
-      <c r="O21" s="23"/>
-      <c r="P21" s="23"/>
-      <c r="Q21" s="23"/>
-      <c r="R21" s="23"/>
+        <v>35</v>
+      </c>
+      <c r="B21" s="6">
+        <v>4461</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" s="17"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="21"/>
+      <c r="J21" s="21"/>
+      <c r="K21" s="21"/>
+      <c r="L21" s="21"/>
+      <c r="M21" s="29"/>
+      <c r="N21" s="29"/>
+      <c r="O21" s="21"/>
+      <c r="P21" s="21"/>
+      <c r="Q21" s="21"/>
+      <c r="R21" s="21"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="B22" s="9"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="22"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="22"/>
-      <c r="I22" s="22"/>
-      <c r="J22" s="22"/>
-      <c r="K22" s="22"/>
-      <c r="L22" s="22"/>
-      <c r="M22" s="31"/>
-      <c r="N22" s="31"/>
-      <c r="O22" s="22"/>
-      <c r="P22" s="22"/>
-      <c r="Q22" s="22"/>
-      <c r="R22" s="22"/>
+        <v>37</v>
+      </c>
+      <c r="B22" s="6">
+        <v>9133</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="21"/>
+      <c r="J22" s="21"/>
+      <c r="K22" s="21"/>
+      <c r="L22" s="21"/>
+      <c r="M22" s="29"/>
+      <c r="N22" s="29"/>
+      <c r="O22" s="21"/>
+      <c r="P22" s="21"/>
+      <c r="Q22" s="21"/>
+      <c r="R22" s="21"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A23" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="B23" s="7"/>
-      <c r="C23" s="8"/>
+      <c r="A23" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" s="9"/>
+      <c r="C23" s="10"/>
       <c r="D23" s="18"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="22"/>
-      <c r="G23" s="22"/>
-      <c r="H23" s="22"/>
-      <c r="I23" s="22"/>
-      <c r="J23" s="22"/>
-      <c r="K23" s="22"/>
-      <c r="L23" s="22"/>
-      <c r="M23" s="31"/>
-      <c r="N23" s="31"/>
-      <c r="O23" s="22"/>
-      <c r="P23" s="22"/>
-      <c r="Q23" s="22"/>
-      <c r="R23" s="22"/>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="G27" s="11"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="18"/>
+      <c r="K23" s="18"/>
+      <c r="L23" s="18"/>
+      <c r="M23" s="18"/>
+      <c r="N23" s="18"/>
+      <c r="O23" s="18"/>
+      <c r="P23" s="18"/>
+      <c r="Q23" s="18"/>
+      <c r="R23" s="18"/>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A24" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" s="9">
+        <v>13266</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" s="24"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="22"/>
+      <c r="I24" s="23"/>
+      <c r="J24" s="23"/>
+      <c r="K24" s="23"/>
+      <c r="L24" s="23"/>
+      <c r="M24" s="30"/>
+      <c r="N24" s="30"/>
+      <c r="O24" s="23"/>
+      <c r="P24" s="23"/>
+      <c r="Q24" s="23"/>
+      <c r="R24" s="23"/>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="G26" s="11"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1942,15 +1986,16 @@
     <hyperlink ref="C15" r:id="rId13" display="mailto:poola.hemalatha@itcinfotech.com" xr:uid="{18898478-C1C3-2848-A308-C0EA55DE3404}"/>
     <hyperlink ref="C16" r:id="rId14" display="mailto:kiran.malali@itcinfotech.com" xr:uid="{E46BD07E-5B3C-6748-B48E-BD29827D1596}"/>
     <hyperlink ref="C17" r:id="rId15" display="mailto:namini.niranjan@itcinfotech.com" xr:uid="{DB79E44B-80D5-0B40-889D-35DAF47CCC6A}"/>
-    <hyperlink ref="C18" r:id="rId16" display="mailto:sheshadri.hejamadi@itcinfotech.com" xr:uid="{919DD6FA-A0ED-4A4E-8EDB-45B028F4B576}"/>
-    <hyperlink ref="C19" r:id="rId17" display="mailto:sreekanth.pidugu@itcinfotech.com" xr:uid="{DDD801BF-A43C-DE4F-AB1C-422062249DE7}"/>
-    <hyperlink ref="C20" r:id="rId18" display="mailto:suresh.ms@itcinfotech.com" xr:uid="{D5EC925E-8FF3-5C41-90AE-2A5AF4655C8E}"/>
-    <hyperlink ref="C21" r:id="rId19" display="mailto:vinod.gvk@itcinfotech.com" xr:uid="{99B4A452-552F-1345-83A8-5AF8CE9B93D9}"/>
+    <hyperlink ref="C20" r:id="rId16" display="mailto:sheshadri.hejamadi@itcinfotech.com" xr:uid="{919DD6FA-A0ED-4A4E-8EDB-45B028F4B576}"/>
+    <hyperlink ref="C21" r:id="rId17" display="mailto:sreekanth.pidugu@itcinfotech.com" xr:uid="{DDD801BF-A43C-DE4F-AB1C-422062249DE7}"/>
+    <hyperlink ref="C22" r:id="rId18" display="mailto:suresh.ms@itcinfotech.com" xr:uid="{D5EC925E-8FF3-5C41-90AE-2A5AF4655C8E}"/>
+    <hyperlink ref="C19" r:id="rId19" xr:uid="{73A92199-9B4B-484F-A18D-116DCEDC6F3C}"/>
+    <hyperlink ref="C24" r:id="rId20" display="mailto:vinod.gvk@itcinfotech.com" xr:uid="{40980A66-21B2-B343-BB89-B5F1270C6729}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
-    <tablePart r:id="rId20"/>
+    <tablePart r:id="rId21"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
attendance as on may 22
</commit_message>
<xml_diff>
--- a/attendance-sheet.xlsx
+++ b/attendance-sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Documents/trainings/general/react/react-itc-may-14-31-2018/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96D36447-5EDD-E448-9D74-3D5C325BC09E}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37EBFA85-BCB8-BD4C-9680-9B881CFFF0B8}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14660" xr2:uid="{CBB9C8E6-5B3B-8049-96F8-54CD5DF45308}"/>
   </bookViews>
@@ -243,7 +243,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -291,6 +291,12 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA9D08E"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="12">
     <border>
@@ -437,7 +443,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -471,7 +477,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="15" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="15" fontId="1" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -487,6 +492,8 @@
     <xf numFmtId="0" fontId="6" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
@@ -1278,7 +1285,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A23" sqref="A23"/>
+      <selection pane="topRight" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1331,10 +1338,10 @@
       <c r="L1" s="13">
         <v>43245</v>
       </c>
-      <c r="M1" s="26">
+      <c r="M1" s="25">
         <v>43246</v>
       </c>
-      <c r="N1" s="26">
+      <c r="N1" s="25">
         <v>43247</v>
       </c>
       <c r="O1" s="13">
@@ -1382,10 +1389,10 @@
       <c r="L2" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="M2" s="27" t="s">
+      <c r="M2" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="N2" s="27" t="s">
+      <c r="N2" s="26" t="s">
         <v>42</v>
       </c>
       <c r="O2" s="15" t="s">
@@ -1412,21 +1419,21 @@
       <c r="C3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="20"/>
-      <c r="M3" s="28"/>
-      <c r="N3" s="28"/>
-      <c r="O3" s="20"/>
-      <c r="P3" s="20"/>
-      <c r="Q3" s="20"/>
-      <c r="R3" s="20"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="27"/>
+      <c r="N3" s="27"/>
+      <c r="O3" s="19"/>
+      <c r="P3" s="19"/>
+      <c r="Q3" s="19"/>
+      <c r="R3" s="19"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
@@ -1438,21 +1445,21 @@
       <c r="C4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="21"/>
-      <c r="J4" s="21"/>
-      <c r="K4" s="21"/>
-      <c r="L4" s="21"/>
-      <c r="M4" s="29"/>
-      <c r="N4" s="29"/>
-      <c r="O4" s="21"/>
-      <c r="P4" s="21"/>
-      <c r="Q4" s="21"/>
-      <c r="R4" s="21"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="28"/>
+      <c r="N4" s="28"/>
+      <c r="O4" s="20"/>
+      <c r="P4" s="20"/>
+      <c r="Q4" s="20"/>
+      <c r="R4" s="20"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
@@ -1464,21 +1471,21 @@
       <c r="C5" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
-      <c r="K5" s="21"/>
-      <c r="L5" s="21"/>
-      <c r="M5" s="29"/>
-      <c r="N5" s="29"/>
-      <c r="O5" s="21"/>
-      <c r="P5" s="21"/>
-      <c r="Q5" s="21"/>
-      <c r="R5" s="21"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="28"/>
+      <c r="N5" s="28"/>
+      <c r="O5" s="20"/>
+      <c r="P5" s="20"/>
+      <c r="Q5" s="20"/>
+      <c r="R5" s="20"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
@@ -1494,17 +1501,17 @@
       <c r="E6" s="17"/>
       <c r="F6" s="17"/>
       <c r="G6" s="17"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="21"/>
-      <c r="K6" s="21"/>
-      <c r="L6" s="21"/>
-      <c r="M6" s="29"/>
-      <c r="N6" s="29"/>
-      <c r="O6" s="21"/>
-      <c r="P6" s="21"/>
-      <c r="Q6" s="21"/>
-      <c r="R6" s="21"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="20"/>
+      <c r="M6" s="28"/>
+      <c r="N6" s="28"/>
+      <c r="O6" s="20"/>
+      <c r="P6" s="20"/>
+      <c r="Q6" s="20"/>
+      <c r="R6" s="20"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
@@ -1517,20 +1524,20 @@
         <v>12</v>
       </c>
       <c r="D7" s="17"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
       <c r="G7" s="18"/>
       <c r="H7" s="18"/>
-      <c r="I7" s="21"/>
-      <c r="J7" s="21"/>
-      <c r="K7" s="21"/>
-      <c r="L7" s="21"/>
-      <c r="M7" s="29"/>
-      <c r="N7" s="29"/>
-      <c r="O7" s="21"/>
-      <c r="P7" s="21"/>
-      <c r="Q7" s="21"/>
-      <c r="R7" s="21"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="20"/>
+      <c r="M7" s="28"/>
+      <c r="N7" s="28"/>
+      <c r="O7" s="20"/>
+      <c r="P7" s="20"/>
+      <c r="Q7" s="20"/>
+      <c r="R7" s="20"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
@@ -1543,20 +1550,20 @@
         <v>14</v>
       </c>
       <c r="D8" s="17"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="21"/>
-      <c r="J8" s="21"/>
-      <c r="K8" s="21"/>
-      <c r="L8" s="21"/>
-      <c r="M8" s="29"/>
-      <c r="N8" s="29"/>
-      <c r="O8" s="21"/>
-      <c r="P8" s="21"/>
-      <c r="Q8" s="21"/>
-      <c r="R8" s="21"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="32"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="28"/>
+      <c r="N8" s="28"/>
+      <c r="O8" s="20"/>
+      <c r="P8" s="20"/>
+      <c r="Q8" s="20"/>
+      <c r="R8" s="20"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
@@ -1569,20 +1576,20 @@
         <v>16</v>
       </c>
       <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
       <c r="G9" s="18"/>
       <c r="H9" s="18"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="21"/>
-      <c r="K9" s="21"/>
-      <c r="L9" s="21"/>
-      <c r="M9" s="29"/>
-      <c r="N9" s="29"/>
-      <c r="O9" s="21"/>
-      <c r="P9" s="21"/>
-      <c r="Q9" s="21"/>
-      <c r="R9" s="21"/>
+      <c r="I9" s="33"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="20"/>
+      <c r="M9" s="28"/>
+      <c r="N9" s="28"/>
+      <c r="O9" s="20"/>
+      <c r="P9" s="20"/>
+      <c r="Q9" s="20"/>
+      <c r="R9" s="20"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
@@ -1594,21 +1601,21 @@
       <c r="C10" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="21"/>
-      <c r="J10" s="21"/>
-      <c r="K10" s="21"/>
-      <c r="L10" s="21"/>
-      <c r="M10" s="29"/>
-      <c r="N10" s="29"/>
-      <c r="O10" s="21"/>
-      <c r="P10" s="21"/>
-      <c r="Q10" s="21"/>
-      <c r="R10" s="21"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="28"/>
+      <c r="N10" s="28"/>
+      <c r="O10" s="20"/>
+      <c r="P10" s="20"/>
+      <c r="Q10" s="20"/>
+      <c r="R10" s="20"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
@@ -1620,21 +1627,21 @@
       <c r="C11" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="18"/>
+      <c r="D11" s="17"/>
       <c r="E11" s="17"/>
       <c r="F11" s="17"/>
       <c r="G11" s="17"/>
       <c r="H11" s="17"/>
-      <c r="I11" s="21"/>
-      <c r="J11" s="21"/>
-      <c r="K11" s="21"/>
-      <c r="L11" s="21"/>
-      <c r="M11" s="29"/>
-      <c r="N11" s="29"/>
-      <c r="O11" s="21"/>
-      <c r="P11" s="21"/>
-      <c r="Q11" s="21"/>
-      <c r="R11" s="21"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="20"/>
+      <c r="M11" s="28"/>
+      <c r="N11" s="28"/>
+      <c r="O11" s="20"/>
+      <c r="P11" s="20"/>
+      <c r="Q11" s="20"/>
+      <c r="R11" s="20"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
@@ -1647,20 +1654,20 @@
         <v>22</v>
       </c>
       <c r="D12" s="17"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="21"/>
-      <c r="J12" s="21"/>
-      <c r="K12" s="21"/>
-      <c r="L12" s="21"/>
-      <c r="M12" s="29"/>
-      <c r="N12" s="29"/>
-      <c r="O12" s="21"/>
-      <c r="P12" s="21"/>
-      <c r="Q12" s="21"/>
-      <c r="R12" s="21"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="20"/>
+      <c r="L12" s="20"/>
+      <c r="M12" s="28"/>
+      <c r="N12" s="28"/>
+      <c r="O12" s="20"/>
+      <c r="P12" s="20"/>
+      <c r="Q12" s="20"/>
+      <c r="R12" s="20"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
@@ -1673,20 +1680,20 @@
         <v>24</v>
       </c>
       <c r="D13" s="17"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
       <c r="G13" s="18"/>
       <c r="H13" s="18"/>
-      <c r="I13" s="21"/>
-      <c r="J13" s="21"/>
-      <c r="K13" s="21"/>
-      <c r="L13" s="21"/>
-      <c r="M13" s="29"/>
-      <c r="N13" s="29"/>
-      <c r="O13" s="21"/>
-      <c r="P13" s="21"/>
-      <c r="Q13" s="21"/>
-      <c r="R13" s="21"/>
+      <c r="I13" s="23"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="20"/>
+      <c r="L13" s="20"/>
+      <c r="M13" s="28"/>
+      <c r="N13" s="28"/>
+      <c r="O13" s="20"/>
+      <c r="P13" s="20"/>
+      <c r="Q13" s="20"/>
+      <c r="R13" s="20"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
@@ -1703,16 +1710,16 @@
       <c r="F14" s="18"/>
       <c r="G14" s="18"/>
       <c r="H14" s="18"/>
-      <c r="I14" s="21"/>
-      <c r="J14" s="21"/>
-      <c r="K14" s="21"/>
-      <c r="L14" s="21"/>
-      <c r="M14" s="29"/>
-      <c r="N14" s="29"/>
-      <c r="O14" s="21"/>
-      <c r="P14" s="21"/>
-      <c r="Q14" s="21"/>
-      <c r="R14" s="21"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="20"/>
+      <c r="L14" s="20"/>
+      <c r="M14" s="28"/>
+      <c r="N14" s="28"/>
+      <c r="O14" s="20"/>
+      <c r="P14" s="20"/>
+      <c r="Q14" s="20"/>
+      <c r="R14" s="20"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
@@ -1724,21 +1731,21 @@
       <c r="C15" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="21"/>
-      <c r="J15" s="21"/>
-      <c r="K15" s="21"/>
-      <c r="L15" s="21"/>
-      <c r="M15" s="29"/>
-      <c r="N15" s="29"/>
-      <c r="O15" s="21"/>
-      <c r="P15" s="21"/>
-      <c r="Q15" s="21"/>
-      <c r="R15" s="21"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="20"/>
+      <c r="L15" s="20"/>
+      <c r="M15" s="28"/>
+      <c r="N15" s="28"/>
+      <c r="O15" s="20"/>
+      <c r="P15" s="20"/>
+      <c r="Q15" s="20"/>
+      <c r="R15" s="20"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
@@ -1751,20 +1758,20 @@
         <v>30</v>
       </c>
       <c r="D16" s="17"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="21"/>
-      <c r="J16" s="21"/>
-      <c r="K16" s="21"/>
-      <c r="L16" s="21"/>
-      <c r="M16" s="29"/>
-      <c r="N16" s="29"/>
-      <c r="O16" s="21"/>
-      <c r="P16" s="21"/>
-      <c r="Q16" s="21"/>
-      <c r="R16" s="21"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="20"/>
+      <c r="L16" s="20"/>
+      <c r="M16" s="28"/>
+      <c r="N16" s="28"/>
+      <c r="O16" s="20"/>
+      <c r="P16" s="20"/>
+      <c r="Q16" s="20"/>
+      <c r="R16" s="20"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
@@ -1777,20 +1784,20 @@
         <v>32</v>
       </c>
       <c r="D17" s="17"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="21"/>
-      <c r="J17" s="21"/>
-      <c r="K17" s="21"/>
-      <c r="L17" s="21"/>
-      <c r="M17" s="29"/>
-      <c r="N17" s="29"/>
-      <c r="O17" s="21"/>
-      <c r="P17" s="21"/>
-      <c r="Q17" s="21"/>
-      <c r="R17" s="21"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="20"/>
+      <c r="K17" s="20"/>
+      <c r="L17" s="20"/>
+      <c r="M17" s="28"/>
+      <c r="N17" s="28"/>
+      <c r="O17" s="20"/>
+      <c r="P17" s="20"/>
+      <c r="Q17" s="20"/>
+      <c r="R17" s="20"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
@@ -1798,21 +1805,21 @@
       </c>
       <c r="B18" s="9"/>
       <c r="C18" s="10"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
-      <c r="K18" s="22"/>
-      <c r="L18" s="22"/>
-      <c r="M18" s="31"/>
-      <c r="N18" s="31"/>
-      <c r="O18" s="22"/>
-      <c r="P18" s="22"/>
-      <c r="Q18" s="22"/>
-      <c r="R18" s="22"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="21"/>
+      <c r="K18" s="21"/>
+      <c r="L18" s="21"/>
+      <c r="M18" s="30"/>
+      <c r="N18" s="30"/>
+      <c r="O18" s="21"/>
+      <c r="P18" s="21"/>
+      <c r="Q18" s="21"/>
+      <c r="R18" s="21"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
@@ -1825,20 +1832,20 @@
         <v>51</v>
       </c>
       <c r="D19" s="18"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="24"/>
-      <c r="H19" s="24"/>
-      <c r="I19" s="22"/>
-      <c r="J19" s="22"/>
-      <c r="K19" s="22"/>
-      <c r="L19" s="22"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="32"/>
+      <c r="J19" s="21"/>
+      <c r="K19" s="21"/>
+      <c r="L19" s="21"/>
       <c r="M19" s="18"/>
       <c r="N19" s="18"/>
-      <c r="O19" s="22"/>
-      <c r="P19" s="22"/>
-      <c r="Q19" s="22"/>
-      <c r="R19" s="22"/>
+      <c r="O19" s="21"/>
+      <c r="P19" s="21"/>
+      <c r="Q19" s="21"/>
+      <c r="R19" s="21"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
@@ -1851,20 +1858,20 @@
         <v>34</v>
       </c>
       <c r="D20" s="17"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="18"/>
-      <c r="I20" s="21"/>
-      <c r="J20" s="21"/>
-      <c r="K20" s="21"/>
-      <c r="L20" s="21"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="32"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="20"/>
+      <c r="L20" s="20"/>
       <c r="M20" s="18"/>
       <c r="N20" s="18"/>
-      <c r="O20" s="21"/>
-      <c r="P20" s="21"/>
-      <c r="Q20" s="21"/>
-      <c r="R20" s="21"/>
+      <c r="O20" s="20"/>
+      <c r="P20" s="20"/>
+      <c r="Q20" s="20"/>
+      <c r="R20" s="20"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
@@ -1877,20 +1884,20 @@
         <v>36</v>
       </c>
       <c r="D21" s="17"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="18"/>
-      <c r="I21" s="21"/>
-      <c r="J21" s="21"/>
-      <c r="K21" s="21"/>
-      <c r="L21" s="21"/>
-      <c r="M21" s="29"/>
-      <c r="N21" s="29"/>
-      <c r="O21" s="21"/>
-      <c r="P21" s="21"/>
-      <c r="Q21" s="21"/>
-      <c r="R21" s="21"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="20"/>
+      <c r="K21" s="20"/>
+      <c r="L21" s="20"/>
+      <c r="M21" s="28"/>
+      <c r="N21" s="28"/>
+      <c r="O21" s="20"/>
+      <c r="P21" s="20"/>
+      <c r="Q21" s="20"/>
+      <c r="R21" s="20"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
@@ -1907,29 +1914,29 @@
       <c r="F22" s="17"/>
       <c r="G22" s="17"/>
       <c r="H22" s="17"/>
-      <c r="I22" s="21"/>
-      <c r="J22" s="21"/>
-      <c r="K22" s="21"/>
-      <c r="L22" s="21"/>
-      <c r="M22" s="29"/>
-      <c r="N22" s="29"/>
-      <c r="O22" s="21"/>
-      <c r="P22" s="21"/>
-      <c r="Q22" s="21"/>
-      <c r="R22" s="21"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="20"/>
+      <c r="K22" s="20"/>
+      <c r="L22" s="20"/>
+      <c r="M22" s="28"/>
+      <c r="N22" s="28"/>
+      <c r="O22" s="20"/>
+      <c r="P22" s="20"/>
+      <c r="Q22" s="20"/>
+      <c r="R22" s="20"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A23" s="32" t="s">
+      <c r="A23" s="31" t="s">
         <v>52</v>
       </c>
       <c r="B23" s="9"/>
       <c r="C23" s="10"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="18"/>
-      <c r="I23" s="18"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="23"/>
+      <c r="I23" s="23"/>
       <c r="J23" s="18"/>
       <c r="K23" s="18"/>
       <c r="L23" s="18"/>
@@ -1950,21 +1957,21 @@
       <c r="C24" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="D24" s="24"/>
-      <c r="E24" s="22"/>
-      <c r="F24" s="22"/>
-      <c r="G24" s="22"/>
-      <c r="H24" s="22"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="23"/>
+      <c r="G24" s="23"/>
+      <c r="H24" s="23"/>
       <c r="I24" s="23"/>
-      <c r="J24" s="23"/>
-      <c r="K24" s="23"/>
-      <c r="L24" s="23"/>
-      <c r="M24" s="30"/>
-      <c r="N24" s="30"/>
-      <c r="O24" s="23"/>
-      <c r="P24" s="23"/>
-      <c r="Q24" s="23"/>
-      <c r="R24" s="23"/>
+      <c r="J24" s="22"/>
+      <c r="K24" s="22"/>
+      <c r="L24" s="22"/>
+      <c r="M24" s="29"/>
+      <c r="N24" s="29"/>
+      <c r="O24" s="22"/>
+      <c r="P24" s="22"/>
+      <c r="Q24" s="22"/>
+      <c r="R24" s="22"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="G26" s="11"/>

</xml_diff>

<commit_message>
after end of may 23 session
</commit_message>
<xml_diff>
--- a/attendance-sheet.xlsx
+++ b/attendance-sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Documents/trainings/general/react/react-itc-may-14-31-2018/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37EBFA85-BCB8-BD4C-9680-9B881CFFF0B8}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D137AA9-037E-6B41-A50D-E5F92FF63A0D}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14660" xr2:uid="{CBB9C8E6-5B3B-8049-96F8-54CD5DF45308}"/>
   </bookViews>
@@ -1285,7 +1285,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E18" sqref="E18"/>
+      <selection pane="topRight" activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1425,7 +1425,7 @@
       <c r="G3" s="17"/>
       <c r="H3" s="17"/>
       <c r="I3" s="17"/>
-      <c r="J3" s="19"/>
+      <c r="J3" s="32"/>
       <c r="K3" s="19"/>
       <c r="L3" s="19"/>
       <c r="M3" s="27"/>
@@ -1451,7 +1451,7 @@
       <c r="G4" s="17"/>
       <c r="H4" s="17"/>
       <c r="I4" s="17"/>
-      <c r="J4" s="20"/>
+      <c r="J4" s="17"/>
       <c r="K4" s="20"/>
       <c r="L4" s="20"/>
       <c r="M4" s="28"/>
@@ -1477,7 +1477,7 @@
       <c r="G5" s="23"/>
       <c r="H5" s="23"/>
       <c r="I5" s="23"/>
-      <c r="J5" s="20"/>
+      <c r="J5" s="32"/>
       <c r="K5" s="20"/>
       <c r="L5" s="20"/>
       <c r="M5" s="28"/>
@@ -1503,7 +1503,7 @@
       <c r="G6" s="17"/>
       <c r="H6" s="17"/>
       <c r="I6" s="32"/>
-      <c r="J6" s="20"/>
+      <c r="J6" s="32"/>
       <c r="K6" s="20"/>
       <c r="L6" s="20"/>
       <c r="M6" s="28"/>
@@ -1529,7 +1529,7 @@
       <c r="G7" s="18"/>
       <c r="H7" s="18"/>
       <c r="I7" s="17"/>
-      <c r="J7" s="20"/>
+      <c r="J7" s="32"/>
       <c r="K7" s="20"/>
       <c r="L7" s="20"/>
       <c r="M7" s="28"/>
@@ -1555,7 +1555,7 @@
       <c r="G8" s="17"/>
       <c r="H8" s="17"/>
       <c r="I8" s="32"/>
-      <c r="J8" s="20"/>
+      <c r="J8" s="32"/>
       <c r="K8" s="20"/>
       <c r="L8" s="20"/>
       <c r="M8" s="28"/>
@@ -1581,7 +1581,7 @@
       <c r="G9" s="18"/>
       <c r="H9" s="18"/>
       <c r="I9" s="33"/>
-      <c r="J9" s="20"/>
+      <c r="J9" s="33"/>
       <c r="K9" s="20"/>
       <c r="L9" s="20"/>
       <c r="M9" s="28"/>
@@ -1633,7 +1633,7 @@
       <c r="G11" s="17"/>
       <c r="H11" s="17"/>
       <c r="I11" s="32"/>
-      <c r="J11" s="20"/>
+      <c r="J11" s="32"/>
       <c r="K11" s="20"/>
       <c r="L11" s="20"/>
       <c r="M11" s="28"/>
@@ -1659,7 +1659,7 @@
       <c r="G12" s="23"/>
       <c r="H12" s="23"/>
       <c r="I12" s="23"/>
-      <c r="J12" s="20"/>
+      <c r="J12" s="32"/>
       <c r="K12" s="20"/>
       <c r="L12" s="20"/>
       <c r="M12" s="28"/>
@@ -1737,7 +1737,7 @@
       <c r="G15" s="17"/>
       <c r="H15" s="17"/>
       <c r="I15" s="17"/>
-      <c r="J15" s="20"/>
+      <c r="J15" s="32"/>
       <c r="K15" s="20"/>
       <c r="L15" s="20"/>
       <c r="M15" s="28"/>
@@ -1763,7 +1763,7 @@
       <c r="G16" s="23"/>
       <c r="H16" s="23"/>
       <c r="I16" s="23"/>
-      <c r="J16" s="20"/>
+      <c r="J16" s="32"/>
       <c r="K16" s="20"/>
       <c r="L16" s="20"/>
       <c r="M16" s="28"/>
@@ -1789,7 +1789,7 @@
       <c r="G17" s="17"/>
       <c r="H17" s="17"/>
       <c r="I17" s="17"/>
-      <c r="J17" s="20"/>
+      <c r="J17" s="17"/>
       <c r="K17" s="20"/>
       <c r="L17" s="20"/>
       <c r="M17" s="28"/>
@@ -1837,7 +1837,7 @@
       <c r="G19" s="23"/>
       <c r="H19" s="23"/>
       <c r="I19" s="32"/>
-      <c r="J19" s="21"/>
+      <c r="J19" s="17"/>
       <c r="K19" s="21"/>
       <c r="L19" s="21"/>
       <c r="M19" s="18"/>
@@ -1863,7 +1863,7 @@
       <c r="G20" s="17"/>
       <c r="H20" s="17"/>
       <c r="I20" s="32"/>
-      <c r="J20" s="20"/>
+      <c r="J20" s="32"/>
       <c r="K20" s="20"/>
       <c r="L20" s="20"/>
       <c r="M20" s="18"/>
@@ -1889,7 +1889,7 @@
       <c r="G21" s="17"/>
       <c r="H21" s="17"/>
       <c r="I21" s="17"/>
-      <c r="J21" s="20"/>
+      <c r="J21" s="32"/>
       <c r="K21" s="20"/>
       <c r="L21" s="20"/>
       <c r="M21" s="28"/>
@@ -1915,7 +1915,7 @@
       <c r="G22" s="17"/>
       <c r="H22" s="17"/>
       <c r="I22" s="17"/>
-      <c r="J22" s="20"/>
+      <c r="J22" s="32"/>
       <c r="K22" s="20"/>
       <c r="L22" s="20"/>
       <c r="M22" s="28"/>
@@ -1937,7 +1937,7 @@
       <c r="G23" s="23"/>
       <c r="H23" s="23"/>
       <c r="I23" s="23"/>
-      <c r="J23" s="18"/>
+      <c r="J23" s="32"/>
       <c r="K23" s="18"/>
       <c r="L23" s="18"/>
       <c r="M23" s="18"/>
@@ -1963,7 +1963,7 @@
       <c r="G24" s="23"/>
       <c r="H24" s="23"/>
       <c r="I24" s="23"/>
-      <c r="J24" s="22"/>
+      <c r="J24" s="32"/>
       <c r="K24" s="22"/>
       <c r="L24" s="22"/>
       <c r="M24" s="29"/>

</xml_diff>

<commit_message>
end of may 24 session
</commit_message>
<xml_diff>
--- a/attendance-sheet.xlsx
+++ b/attendance-sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Documents/trainings/general/react/react-itc-may-14-31-2018/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D137AA9-037E-6B41-A50D-E5F92FF63A0D}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C793832-F9B4-E845-9F7A-65DA9C0E510D}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14660" xr2:uid="{CBB9C8E6-5B3B-8049-96F8-54CD5DF45308}"/>
   </bookViews>
@@ -1285,7 +1285,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J10" sqref="J10"/>
+      <selection pane="topRight" activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1426,7 +1426,7 @@
       <c r="H3" s="17"/>
       <c r="I3" s="17"/>
       <c r="J3" s="32"/>
-      <c r="K3" s="19"/>
+      <c r="K3" s="32"/>
       <c r="L3" s="19"/>
       <c r="M3" s="27"/>
       <c r="N3" s="27"/>
@@ -1452,7 +1452,7 @@
       <c r="H4" s="17"/>
       <c r="I4" s="17"/>
       <c r="J4" s="17"/>
-      <c r="K4" s="20"/>
+      <c r="K4" s="32"/>
       <c r="L4" s="20"/>
       <c r="M4" s="28"/>
       <c r="N4" s="28"/>
@@ -1478,7 +1478,7 @@
       <c r="H5" s="23"/>
       <c r="I5" s="23"/>
       <c r="J5" s="32"/>
-      <c r="K5" s="20"/>
+      <c r="K5" s="32"/>
       <c r="L5" s="20"/>
       <c r="M5" s="28"/>
       <c r="N5" s="28"/>
@@ -1504,7 +1504,7 @@
       <c r="H6" s="17"/>
       <c r="I6" s="32"/>
       <c r="J6" s="32"/>
-      <c r="K6" s="20"/>
+      <c r="K6" s="32"/>
       <c r="L6" s="20"/>
       <c r="M6" s="28"/>
       <c r="N6" s="28"/>
@@ -1530,7 +1530,7 @@
       <c r="H7" s="18"/>
       <c r="I7" s="17"/>
       <c r="J7" s="32"/>
-      <c r="K7" s="20"/>
+      <c r="K7" s="17"/>
       <c r="L7" s="20"/>
       <c r="M7" s="28"/>
       <c r="N7" s="28"/>
@@ -1556,7 +1556,7 @@
       <c r="H8" s="17"/>
       <c r="I8" s="32"/>
       <c r="J8" s="32"/>
-      <c r="K8" s="20"/>
+      <c r="K8" s="17"/>
       <c r="L8" s="20"/>
       <c r="M8" s="28"/>
       <c r="N8" s="28"/>
@@ -1582,7 +1582,7 @@
       <c r="H9" s="18"/>
       <c r="I9" s="33"/>
       <c r="J9" s="33"/>
-      <c r="K9" s="20"/>
+      <c r="K9" s="33"/>
       <c r="L9" s="20"/>
       <c r="M9" s="28"/>
       <c r="N9" s="28"/>
@@ -1634,7 +1634,7 @@
       <c r="H11" s="17"/>
       <c r="I11" s="32"/>
       <c r="J11" s="32"/>
-      <c r="K11" s="20"/>
+      <c r="K11" s="17"/>
       <c r="L11" s="20"/>
       <c r="M11" s="28"/>
       <c r="N11" s="28"/>
@@ -1660,7 +1660,7 @@
       <c r="H12" s="23"/>
       <c r="I12" s="23"/>
       <c r="J12" s="32"/>
-      <c r="K12" s="20"/>
+      <c r="K12" s="17"/>
       <c r="L12" s="20"/>
       <c r="M12" s="28"/>
       <c r="N12" s="28"/>
@@ -1738,7 +1738,7 @@
       <c r="H15" s="17"/>
       <c r="I15" s="17"/>
       <c r="J15" s="32"/>
-      <c r="K15" s="20"/>
+      <c r="K15" s="32"/>
       <c r="L15" s="20"/>
       <c r="M15" s="28"/>
       <c r="N15" s="28"/>
@@ -1764,7 +1764,7 @@
       <c r="H16" s="23"/>
       <c r="I16" s="23"/>
       <c r="J16" s="32"/>
-      <c r="K16" s="20"/>
+      <c r="K16" s="32"/>
       <c r="L16" s="20"/>
       <c r="M16" s="28"/>
       <c r="N16" s="28"/>
@@ -1790,7 +1790,7 @@
       <c r="H17" s="17"/>
       <c r="I17" s="17"/>
       <c r="J17" s="17"/>
-      <c r="K17" s="20"/>
+      <c r="K17" s="32"/>
       <c r="L17" s="20"/>
       <c r="M17" s="28"/>
       <c r="N17" s="28"/>
@@ -1838,7 +1838,7 @@
       <c r="H19" s="23"/>
       <c r="I19" s="32"/>
       <c r="J19" s="17"/>
-      <c r="K19" s="21"/>
+      <c r="K19" s="17"/>
       <c r="L19" s="21"/>
       <c r="M19" s="18"/>
       <c r="N19" s="18"/>
@@ -1864,7 +1864,7 @@
       <c r="H20" s="17"/>
       <c r="I20" s="32"/>
       <c r="J20" s="32"/>
-      <c r="K20" s="20"/>
+      <c r="K20" s="17"/>
       <c r="L20" s="20"/>
       <c r="M20" s="18"/>
       <c r="N20" s="18"/>
@@ -1890,7 +1890,7 @@
       <c r="H21" s="17"/>
       <c r="I21" s="17"/>
       <c r="J21" s="32"/>
-      <c r="K21" s="20"/>
+      <c r="K21" s="17"/>
       <c r="L21" s="20"/>
       <c r="M21" s="28"/>
       <c r="N21" s="28"/>
@@ -1916,7 +1916,7 @@
       <c r="H22" s="17"/>
       <c r="I22" s="17"/>
       <c r="J22" s="32"/>
-      <c r="K22" s="20"/>
+      <c r="K22" s="17"/>
       <c r="L22" s="20"/>
       <c r="M22" s="28"/>
       <c r="N22" s="28"/>
@@ -1938,7 +1938,7 @@
       <c r="H23" s="23"/>
       <c r="I23" s="23"/>
       <c r="J23" s="32"/>
-      <c r="K23" s="18"/>
+      <c r="K23" s="32"/>
       <c r="L23" s="18"/>
       <c r="M23" s="18"/>
       <c r="N23" s="18"/>

</xml_diff>

<commit_message>
after end of may 25 session
</commit_message>
<xml_diff>
--- a/attendance-sheet.xlsx
+++ b/attendance-sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Documents/trainings/general/react/react-itc-may-14-31-2018/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A7C31B3-AA10-7249-8D33-CDDB3E569D5A}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F134097-C801-7D41-80AA-D07BBE8AB975}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14660" xr2:uid="{CBB9C8E6-5B3B-8049-96F8-54CD5DF45308}"/>
   </bookViews>
@@ -1285,7 +1285,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L23" sqref="L23"/>
+      <selection pane="topRight" activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1583,7 +1583,7 @@
       <c r="I9" s="33"/>
       <c r="J9" s="33"/>
       <c r="K9" s="33"/>
-      <c r="L9" s="20"/>
+      <c r="L9" s="33"/>
       <c r="M9" s="28"/>
       <c r="N9" s="28"/>
       <c r="O9" s="20"/>
@@ -1765,7 +1765,7 @@
       <c r="I16" s="23"/>
       <c r="J16" s="32"/>
       <c r="K16" s="32"/>
-      <c r="L16" s="20"/>
+      <c r="L16" s="32"/>
       <c r="M16" s="28"/>
       <c r="N16" s="28"/>
       <c r="O16" s="20"/>

</xml_diff>

<commit_message>
end of may 28 session
</commit_message>
<xml_diff>
--- a/attendance-sheet.xlsx
+++ b/attendance-sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Documents/trainings/general/react/react-itc-may-14-31-2018/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77B29CB9-BA05-0B45-B88D-63F764068A0E}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C551816-F405-394C-B568-9267BC29E68E}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14660" xr2:uid="{CBB9C8E6-5B3B-8049-96F8-54CD5DF45308}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="53">
   <si>
     <t>PS ID</t>
   </si>
@@ -443,7 +443,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -487,7 +487,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="22" fontId="6" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="15" fontId="6" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1281,11 +1280,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8890E798-F38F-8643-943F-E0FFFE37A055}">
-  <dimension ref="A1:S26"/>
+  <dimension ref="A1:R26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M17" sqref="M17"/>
+      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1297,11 +1296,11 @@
     <col min="5" max="6" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="12" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="18" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="17" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
         <v>1</v>
       </c>
@@ -1341,24 +1340,21 @@
       <c r="M1" s="25">
         <v>43246</v>
       </c>
-      <c r="N1" s="25">
-        <v>43247</v>
+      <c r="N1" s="13">
+        <v>43248</v>
       </c>
       <c r="O1" s="13">
-        <v>43248</v>
+        <v>43249</v>
       </c>
       <c r="P1" s="13">
-        <v>43249</v>
+        <v>43250</v>
       </c>
       <c r="Q1" s="13">
-        <v>43250</v>
-      </c>
-      <c r="R1" s="13">
         <v>43251</v>
       </c>
-      <c r="S1" s="1"/>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="R1" s="1"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
       <c r="B2" s="4"/>
       <c r="C2" s="5"/>
@@ -1392,8 +1388,8 @@
       <c r="M2" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="N2" s="26" t="s">
-        <v>42</v>
+      <c r="N2" s="15" t="s">
+        <v>41</v>
       </c>
       <c r="O2" s="15" t="s">
         <v>41</v>
@@ -1404,12 +1400,9 @@
       <c r="Q2" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="R2" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="S2" s="1"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="R2" s="1"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>3</v>
       </c>
@@ -1425,17 +1418,16 @@
       <c r="G3" s="17"/>
       <c r="H3" s="17"/>
       <c r="I3" s="17"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="32"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
       <c r="L3" s="17"/>
       <c r="M3" s="17"/>
-      <c r="N3" s="27"/>
+      <c r="N3" s="17"/>
       <c r="O3" s="19"/>
       <c r="P3" s="19"/>
       <c r="Q3" s="19"/>
-      <c r="R3" s="19"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>5</v>
       </c>
@@ -1452,16 +1444,15 @@
       <c r="H4" s="17"/>
       <c r="I4" s="17"/>
       <c r="J4" s="17"/>
-      <c r="K4" s="32"/>
+      <c r="K4" s="31"/>
       <c r="L4" s="17"/>
       <c r="M4" s="17"/>
-      <c r="N4" s="28"/>
+      <c r="N4" s="17"/>
       <c r="O4" s="20"/>
       <c r="P4" s="20"/>
       <c r="Q4" s="20"/>
-      <c r="R4" s="20"/>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>7</v>
       </c>
@@ -1477,17 +1468,16 @@
       <c r="G5" s="23"/>
       <c r="H5" s="23"/>
       <c r="I5" s="23"/>
-      <c r="J5" s="32"/>
-      <c r="K5" s="32"/>
+      <c r="J5" s="31"/>
+      <c r="K5" s="31"/>
       <c r="L5" s="20"/>
-      <c r="M5" s="28"/>
-      <c r="N5" s="28"/>
+      <c r="M5" s="27"/>
+      <c r="N5" s="17"/>
       <c r="O5" s="20"/>
       <c r="P5" s="20"/>
       <c r="Q5" s="20"/>
-      <c r="R5" s="20"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>9</v>
       </c>
@@ -1502,18 +1492,17 @@
       <c r="F6" s="17"/>
       <c r="G6" s="17"/>
       <c r="H6" s="17"/>
-      <c r="I6" s="32"/>
-      <c r="J6" s="32"/>
-      <c r="K6" s="32"/>
-      <c r="L6" s="32"/>
+      <c r="I6" s="31"/>
+      <c r="J6" s="31"/>
+      <c r="K6" s="31"/>
+      <c r="L6" s="31"/>
       <c r="M6" s="17"/>
-      <c r="N6" s="28"/>
+      <c r="N6" s="20"/>
       <c r="O6" s="20"/>
       <c r="P6" s="20"/>
       <c r="Q6" s="20"/>
-      <c r="R6" s="20"/>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
@@ -1529,17 +1518,16 @@
       <c r="G7" s="18"/>
       <c r="H7" s="18"/>
       <c r="I7" s="17"/>
-      <c r="J7" s="32"/>
+      <c r="J7" s="31"/>
       <c r="K7" s="17"/>
-      <c r="L7" s="32"/>
+      <c r="L7" s="31"/>
       <c r="M7" s="17"/>
-      <c r="N7" s="28"/>
+      <c r="N7" s="17"/>
       <c r="O7" s="20"/>
       <c r="P7" s="20"/>
       <c r="Q7" s="20"/>
-      <c r="R7" s="20"/>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>13</v>
       </c>
@@ -1554,18 +1542,17 @@
       <c r="F8" s="17"/>
       <c r="G8" s="17"/>
       <c r="H8" s="17"/>
-      <c r="I8" s="32"/>
-      <c r="J8" s="32"/>
+      <c r="I8" s="31"/>
+      <c r="J8" s="31"/>
       <c r="K8" s="17"/>
       <c r="L8" s="17"/>
       <c r="M8" s="17"/>
-      <c r="N8" s="28"/>
+      <c r="N8" s="17"/>
       <c r="O8" s="20"/>
       <c r="P8" s="20"/>
       <c r="Q8" s="20"/>
-      <c r="R8" s="20"/>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>15</v>
       </c>
@@ -1576,22 +1563,21 @@
         <v>16</v>
       </c>
       <c r="D9" s="18"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
       <c r="G9" s="18"/>
       <c r="H9" s="18"/>
-      <c r="I9" s="33"/>
-      <c r="J9" s="33"/>
-      <c r="K9" s="33"/>
-      <c r="L9" s="33"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="32"/>
+      <c r="L9" s="32"/>
       <c r="M9" s="17"/>
-      <c r="N9" s="28"/>
+      <c r="N9" s="17"/>
       <c r="O9" s="20"/>
       <c r="P9" s="20"/>
       <c r="Q9" s="20"/>
-      <c r="R9" s="20"/>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>17</v>
       </c>
@@ -1601,23 +1587,22 @@
       <c r="C10" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="33"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="33"/>
-      <c r="H10" s="33"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="32"/>
       <c r="I10" s="20"/>
       <c r="J10" s="20"/>
       <c r="K10" s="20"/>
       <c r="L10" s="20"/>
-      <c r="M10" s="28"/>
-      <c r="N10" s="28"/>
+      <c r="M10" s="27"/>
+      <c r="N10" s="20"/>
       <c r="O10" s="20"/>
       <c r="P10" s="20"/>
       <c r="Q10" s="20"/>
-      <c r="R10" s="20"/>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>19</v>
       </c>
@@ -1632,18 +1617,17 @@
       <c r="F11" s="17"/>
       <c r="G11" s="17"/>
       <c r="H11" s="17"/>
-      <c r="I11" s="32"/>
-      <c r="J11" s="32"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="31"/>
       <c r="K11" s="17"/>
       <c r="L11" s="17"/>
-      <c r="M11" s="28"/>
-      <c r="N11" s="28"/>
+      <c r="M11" s="27"/>
+      <c r="N11" s="17"/>
       <c r="O11" s="20"/>
       <c r="P11" s="20"/>
       <c r="Q11" s="20"/>
-      <c r="R11" s="20"/>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>21</v>
       </c>
@@ -1659,17 +1643,16 @@
       <c r="G12" s="23"/>
       <c r="H12" s="23"/>
       <c r="I12" s="23"/>
-      <c r="J12" s="32"/>
+      <c r="J12" s="31"/>
       <c r="K12" s="17"/>
       <c r="L12" s="20"/>
       <c r="M12" s="17"/>
-      <c r="N12" s="28"/>
+      <c r="N12" s="17"/>
       <c r="O12" s="20"/>
       <c r="P12" s="20"/>
       <c r="Q12" s="20"/>
-      <c r="R12" s="20"/>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>23</v>
       </c>
@@ -1688,14 +1671,13 @@
       <c r="J13" s="20"/>
       <c r="K13" s="20"/>
       <c r="L13" s="17"/>
-      <c r="M13" s="28"/>
-      <c r="N13" s="28"/>
+      <c r="M13" s="27"/>
+      <c r="N13" s="17"/>
       <c r="O13" s="20"/>
       <c r="P13" s="20"/>
       <c r="Q13" s="20"/>
-      <c r="R13" s="20"/>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>25</v>
       </c>
@@ -1714,14 +1696,13 @@
       <c r="J14" s="20"/>
       <c r="K14" s="20"/>
       <c r="L14" s="20"/>
-      <c r="M14" s="28"/>
-      <c r="N14" s="28"/>
+      <c r="M14" s="27"/>
+      <c r="N14" s="20"/>
       <c r="O14" s="20"/>
       <c r="P14" s="20"/>
       <c r="Q14" s="20"/>
-      <c r="R14" s="20"/>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
         <v>27</v>
       </c>
@@ -1737,17 +1718,16 @@
       <c r="G15" s="17"/>
       <c r="H15" s="17"/>
       <c r="I15" s="17"/>
-      <c r="J15" s="32"/>
-      <c r="K15" s="32"/>
-      <c r="L15" s="32"/>
+      <c r="J15" s="31"/>
+      <c r="K15" s="31"/>
+      <c r="L15" s="31"/>
       <c r="M15" s="17"/>
-      <c r="N15" s="28"/>
+      <c r="N15" s="20"/>
       <c r="O15" s="20"/>
       <c r="P15" s="20"/>
       <c r="Q15" s="20"/>
-      <c r="R15" s="20"/>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>29</v>
       </c>
@@ -1763,17 +1743,16 @@
       <c r="G16" s="23"/>
       <c r="H16" s="23"/>
       <c r="I16" s="23"/>
-      <c r="J16" s="32"/>
-      <c r="K16" s="32"/>
-      <c r="L16" s="32"/>
+      <c r="J16" s="31"/>
+      <c r="K16" s="31"/>
+      <c r="L16" s="31"/>
       <c r="M16" s="17"/>
-      <c r="N16" s="28"/>
+      <c r="N16" s="17"/>
       <c r="O16" s="20"/>
       <c r="P16" s="20"/>
       <c r="Q16" s="20"/>
-      <c r="R16" s="20"/>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>31</v>
       </c>
@@ -1790,16 +1769,15 @@
       <c r="H17" s="17"/>
       <c r="I17" s="17"/>
       <c r="J17" s="17"/>
-      <c r="K17" s="32"/>
+      <c r="K17" s="31"/>
       <c r="L17" s="17"/>
       <c r="M17" s="17"/>
-      <c r="N17" s="28"/>
+      <c r="N17" s="17"/>
       <c r="O17" s="20"/>
       <c r="P17" s="20"/>
       <c r="Q17" s="20"/>
-      <c r="R17" s="20"/>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>49</v>
       </c>
@@ -1814,14 +1792,13 @@
       <c r="J18" s="21"/>
       <c r="K18" s="21"/>
       <c r="L18" s="21"/>
-      <c r="M18" s="30"/>
-      <c r="N18" s="30"/>
+      <c r="M18" s="29"/>
+      <c r="N18" s="21"/>
       <c r="O18" s="21"/>
       <c r="P18" s="21"/>
       <c r="Q18" s="21"/>
-      <c r="R18" s="21"/>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>50</v>
       </c>
@@ -1836,18 +1813,17 @@
       <c r="F19" s="23"/>
       <c r="G19" s="23"/>
       <c r="H19" s="23"/>
-      <c r="I19" s="32"/>
+      <c r="I19" s="31"/>
       <c r="J19" s="17"/>
       <c r="K19" s="17"/>
       <c r="L19" s="21"/>
       <c r="M19" s="17"/>
-      <c r="N19" s="18"/>
+      <c r="N19" s="17"/>
       <c r="O19" s="21"/>
       <c r="P19" s="21"/>
       <c r="Q19" s="21"/>
-      <c r="R19" s="21"/>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
         <v>33</v>
       </c>
@@ -1862,18 +1838,17 @@
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
       <c r="H20" s="17"/>
-      <c r="I20" s="32"/>
-      <c r="J20" s="32"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
       <c r="K20" s="17"/>
-      <c r="L20" s="32"/>
+      <c r="L20" s="31"/>
       <c r="M20" s="17"/>
-      <c r="N20" s="18"/>
+      <c r="N20" s="20"/>
       <c r="O20" s="20"/>
       <c r="P20" s="20"/>
       <c r="Q20" s="20"/>
-      <c r="R20" s="20"/>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
         <v>35</v>
       </c>
@@ -1889,17 +1864,16 @@
       <c r="G21" s="17"/>
       <c r="H21" s="17"/>
       <c r="I21" s="17"/>
-      <c r="J21" s="32"/>
+      <c r="J21" s="31"/>
       <c r="K21" s="17"/>
       <c r="L21" s="17"/>
-      <c r="M21" s="28"/>
-      <c r="N21" s="28"/>
+      <c r="M21" s="27"/>
+      <c r="N21" s="17"/>
       <c r="O21" s="20"/>
       <c r="P21" s="20"/>
       <c r="Q21" s="20"/>
-      <c r="R21" s="20"/>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
         <v>37</v>
       </c>
@@ -1915,18 +1889,17 @@
       <c r="G22" s="17"/>
       <c r="H22" s="17"/>
       <c r="I22" s="17"/>
-      <c r="J22" s="32"/>
+      <c r="J22" s="31"/>
       <c r="K22" s="17"/>
       <c r="L22" s="17"/>
       <c r="M22" s="17"/>
-      <c r="N22" s="28"/>
+      <c r="N22" s="17"/>
       <c r="O22" s="20"/>
       <c r="P22" s="20"/>
       <c r="Q22" s="20"/>
-      <c r="R22" s="20"/>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A23" s="31" t="s">
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A23" s="30" t="s">
         <v>52</v>
       </c>
       <c r="B23" s="9"/>
@@ -1937,17 +1910,16 @@
       <c r="G23" s="23"/>
       <c r="H23" s="23"/>
       <c r="I23" s="23"/>
-      <c r="J23" s="32"/>
-      <c r="K23" s="32"/>
+      <c r="J23" s="31"/>
+      <c r="K23" s="31"/>
       <c r="L23" s="17"/>
       <c r="M23" s="17"/>
-      <c r="N23" s="18"/>
+      <c r="N23" s="17"/>
       <c r="O23" s="18"/>
       <c r="P23" s="18"/>
       <c r="Q23" s="18"/>
-      <c r="R23" s="18"/>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
         <v>39</v>
       </c>
@@ -1963,17 +1935,16 @@
       <c r="G24" s="23"/>
       <c r="H24" s="23"/>
       <c r="I24" s="23"/>
-      <c r="J24" s="32"/>
+      <c r="J24" s="31"/>
       <c r="K24" s="22"/>
       <c r="L24" s="22"/>
-      <c r="M24" s="29"/>
-      <c r="N24" s="29"/>
+      <c r="M24" s="28"/>
+      <c r="N24" s="17"/>
       <c r="O24" s="22"/>
       <c r="P24" s="22"/>
       <c r="Q24" s="22"/>
-      <c r="R24" s="22"/>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="G26" s="11"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
after end of may 29 session
</commit_message>
<xml_diff>
--- a/attendance-sheet.xlsx
+++ b/attendance-sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Documents/trainings/general/react/react-itc-may-14-31-2018/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C551816-F405-394C-B568-9267BC29E68E}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{A7A1BB9D-65FA-814D-961D-101859376779}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14660" xr2:uid="{CBB9C8E6-5B3B-8049-96F8-54CD5DF45308}"/>
   </bookViews>
@@ -1284,7 +1284,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N16" sqref="N16"/>
+      <selection pane="topRight" activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1423,7 +1423,7 @@
       <c r="L3" s="17"/>
       <c r="M3" s="17"/>
       <c r="N3" s="17"/>
-      <c r="O3" s="19"/>
+      <c r="O3" s="17"/>
       <c r="P3" s="19"/>
       <c r="Q3" s="19"/>
     </row>
@@ -1448,7 +1448,7 @@
       <c r="L4" s="17"/>
       <c r="M4" s="17"/>
       <c r="N4" s="17"/>
-      <c r="O4" s="20"/>
+      <c r="O4" s="17"/>
       <c r="P4" s="20"/>
       <c r="Q4" s="20"/>
     </row>
@@ -1473,7 +1473,7 @@
       <c r="L5" s="20"/>
       <c r="M5" s="27"/>
       <c r="N5" s="17"/>
-      <c r="O5" s="20"/>
+      <c r="O5" s="17"/>
       <c r="P5" s="20"/>
       <c r="Q5" s="20"/>
     </row>
@@ -1498,7 +1498,7 @@
       <c r="L6" s="31"/>
       <c r="M6" s="17"/>
       <c r="N6" s="20"/>
-      <c r="O6" s="20"/>
+      <c r="O6" s="17"/>
       <c r="P6" s="20"/>
       <c r="Q6" s="20"/>
     </row>
@@ -1523,7 +1523,7 @@
       <c r="L7" s="31"/>
       <c r="M7" s="17"/>
       <c r="N7" s="17"/>
-      <c r="O7" s="20"/>
+      <c r="O7" s="17"/>
       <c r="P7" s="20"/>
       <c r="Q7" s="20"/>
     </row>
@@ -1548,7 +1548,7 @@
       <c r="L8" s="17"/>
       <c r="M8" s="17"/>
       <c r="N8" s="17"/>
-      <c r="O8" s="20"/>
+      <c r="O8" s="17"/>
       <c r="P8" s="20"/>
       <c r="Q8" s="20"/>
     </row>
@@ -1598,7 +1598,7 @@
       <c r="L10" s="20"/>
       <c r="M10" s="27"/>
       <c r="N10" s="20"/>
-      <c r="O10" s="20"/>
+      <c r="O10" s="17"/>
       <c r="P10" s="20"/>
       <c r="Q10" s="20"/>
     </row>
@@ -1623,7 +1623,7 @@
       <c r="L11" s="17"/>
       <c r="M11" s="27"/>
       <c r="N11" s="17"/>
-      <c r="O11" s="20"/>
+      <c r="O11" s="17"/>
       <c r="P11" s="20"/>
       <c r="Q11" s="20"/>
     </row>
@@ -1648,7 +1648,7 @@
       <c r="L12" s="20"/>
       <c r="M12" s="17"/>
       <c r="N12" s="17"/>
-      <c r="O12" s="20"/>
+      <c r="O12" s="17"/>
       <c r="P12" s="20"/>
       <c r="Q12" s="20"/>
     </row>
@@ -1673,7 +1673,7 @@
       <c r="L13" s="17"/>
       <c r="M13" s="27"/>
       <c r="N13" s="17"/>
-      <c r="O13" s="20"/>
+      <c r="O13" s="17"/>
       <c r="P13" s="20"/>
       <c r="Q13" s="20"/>
     </row>
@@ -1723,7 +1723,7 @@
       <c r="L15" s="31"/>
       <c r="M15" s="17"/>
       <c r="N15" s="20"/>
-      <c r="O15" s="20"/>
+      <c r="O15" s="17"/>
       <c r="P15" s="20"/>
       <c r="Q15" s="20"/>
     </row>
@@ -1748,7 +1748,7 @@
       <c r="L16" s="31"/>
       <c r="M16" s="17"/>
       <c r="N16" s="17"/>
-      <c r="O16" s="20"/>
+      <c r="O16" s="17"/>
       <c r="P16" s="20"/>
       <c r="Q16" s="20"/>
     </row>
@@ -1773,7 +1773,7 @@
       <c r="L17" s="17"/>
       <c r="M17" s="17"/>
       <c r="N17" s="17"/>
-      <c r="O17" s="20"/>
+      <c r="O17" s="17"/>
       <c r="P17" s="20"/>
       <c r="Q17" s="20"/>
     </row>
@@ -1819,7 +1819,7 @@
       <c r="L19" s="21"/>
       <c r="M19" s="17"/>
       <c r="N19" s="17"/>
-      <c r="O19" s="21"/>
+      <c r="O19" s="17"/>
       <c r="P19" s="21"/>
       <c r="Q19" s="21"/>
     </row>
@@ -1869,7 +1869,7 @@
       <c r="L21" s="17"/>
       <c r="M21" s="27"/>
       <c r="N21" s="17"/>
-      <c r="O21" s="20"/>
+      <c r="O21" s="17"/>
       <c r="P21" s="20"/>
       <c r="Q21" s="20"/>
     </row>
@@ -1894,7 +1894,7 @@
       <c r="L22" s="17"/>
       <c r="M22" s="17"/>
       <c r="N22" s="17"/>
-      <c r="O22" s="20"/>
+      <c r="O22" s="17"/>
       <c r="P22" s="20"/>
       <c r="Q22" s="20"/>
     </row>
@@ -1915,7 +1915,7 @@
       <c r="L23" s="17"/>
       <c r="M23" s="17"/>
       <c r="N23" s="17"/>
-      <c r="O23" s="18"/>
+      <c r="O23" s="17"/>
       <c r="P23" s="18"/>
       <c r="Q23" s="18"/>
     </row>
@@ -1940,7 +1940,7 @@
       <c r="L24" s="22"/>
       <c r="M24" s="28"/>
       <c r="N24" s="17"/>
-      <c r="O24" s="22"/>
+      <c r="O24" s="17"/>
       <c r="P24" s="22"/>
       <c r="Q24" s="22"/>
     </row>

</xml_diff>

<commit_message>
after end of may 30 session
</commit_message>
<xml_diff>
--- a/attendance-sheet.xlsx
+++ b/attendance-sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Documents/trainings/general/react/react-itc-may-14-31-2018/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{A7A1BB9D-65FA-814D-961D-101859376779}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89375018-FB85-6C45-8EF6-E393C0FB5931}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14660" xr2:uid="{CBB9C8E6-5B3B-8049-96F8-54CD5DF45308}"/>
   </bookViews>
@@ -1283,8 +1283,8 @@
   <dimension ref="A1:R26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="O5" sqref="O5"/>
+      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="P24" sqref="P24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1424,7 +1424,7 @@
       <c r="M3" s="17"/>
       <c r="N3" s="17"/>
       <c r="O3" s="17"/>
-      <c r="P3" s="19"/>
+      <c r="P3" s="17"/>
       <c r="Q3" s="19"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
@@ -1449,7 +1449,7 @@
       <c r="M4" s="17"/>
       <c r="N4" s="17"/>
       <c r="O4" s="17"/>
-      <c r="P4" s="20"/>
+      <c r="P4" s="17"/>
       <c r="Q4" s="20"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
@@ -1474,7 +1474,7 @@
       <c r="M5" s="27"/>
       <c r="N5" s="17"/>
       <c r="O5" s="17"/>
-      <c r="P5" s="20"/>
+      <c r="P5" s="17"/>
       <c r="Q5" s="20"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
@@ -1499,7 +1499,7 @@
       <c r="M6" s="17"/>
       <c r="N6" s="20"/>
       <c r="O6" s="17"/>
-      <c r="P6" s="20"/>
+      <c r="P6" s="17"/>
       <c r="Q6" s="20"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
@@ -1524,7 +1524,7 @@
       <c r="M7" s="17"/>
       <c r="N7" s="17"/>
       <c r="O7" s="17"/>
-      <c r="P7" s="20"/>
+      <c r="P7" s="17"/>
       <c r="Q7" s="20"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
@@ -1549,7 +1549,7 @@
       <c r="M8" s="17"/>
       <c r="N8" s="17"/>
       <c r="O8" s="17"/>
-      <c r="P8" s="20"/>
+      <c r="P8" s="17"/>
       <c r="Q8" s="20"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
@@ -1573,8 +1573,8 @@
       <c r="L9" s="32"/>
       <c r="M9" s="17"/>
       <c r="N9" s="17"/>
-      <c r="O9" s="20"/>
-      <c r="P9" s="20"/>
+      <c r="O9" s="17"/>
+      <c r="P9" s="17"/>
       <c r="Q9" s="20"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
@@ -1599,7 +1599,7 @@
       <c r="M10" s="27"/>
       <c r="N10" s="20"/>
       <c r="O10" s="17"/>
-      <c r="P10" s="20"/>
+      <c r="P10" s="17"/>
       <c r="Q10" s="20"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
@@ -1674,7 +1674,7 @@
       <c r="M13" s="27"/>
       <c r="N13" s="17"/>
       <c r="O13" s="17"/>
-      <c r="P13" s="20"/>
+      <c r="P13" s="17"/>
       <c r="Q13" s="20"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
@@ -1724,7 +1724,7 @@
       <c r="M15" s="17"/>
       <c r="N15" s="20"/>
       <c r="O15" s="17"/>
-      <c r="P15" s="20"/>
+      <c r="P15" s="17"/>
       <c r="Q15" s="20"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
@@ -1749,7 +1749,7 @@
       <c r="M16" s="17"/>
       <c r="N16" s="17"/>
       <c r="O16" s="17"/>
-      <c r="P16" s="20"/>
+      <c r="P16" s="17"/>
       <c r="Q16" s="20"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.2">
@@ -1774,7 +1774,7 @@
       <c r="M17" s="17"/>
       <c r="N17" s="17"/>
       <c r="O17" s="17"/>
-      <c r="P17" s="20"/>
+      <c r="P17" s="17"/>
       <c r="Q17" s="20"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.2">
@@ -1845,7 +1845,7 @@
       <c r="M20" s="17"/>
       <c r="N20" s="20"/>
       <c r="O20" s="20"/>
-      <c r="P20" s="20"/>
+      <c r="P20" s="17"/>
       <c r="Q20" s="20"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.2">
@@ -1870,7 +1870,7 @@
       <c r="M21" s="27"/>
       <c r="N21" s="17"/>
       <c r="O21" s="17"/>
-      <c r="P21" s="20"/>
+      <c r="P21" s="17"/>
       <c r="Q21" s="20"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.2">
@@ -1895,7 +1895,7 @@
       <c r="M22" s="17"/>
       <c r="N22" s="17"/>
       <c r="O22" s="17"/>
-      <c r="P22" s="20"/>
+      <c r="P22" s="17"/>
       <c r="Q22" s="20"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.2">
@@ -1916,7 +1916,7 @@
       <c r="M23" s="17"/>
       <c r="N23" s="17"/>
       <c r="O23" s="17"/>
-      <c r="P23" s="18"/>
+      <c r="P23" s="17"/>
       <c r="Q23" s="18"/>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.2">
@@ -1941,7 +1941,7 @@
       <c r="M24" s="28"/>
       <c r="N24" s="17"/>
       <c r="O24" s="17"/>
-      <c r="P24" s="22"/>
+      <c r="P24" s="17"/>
       <c r="Q24" s="22"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
after end of may 31 session
</commit_message>
<xml_diff>
--- a/attendance-sheet.xlsx
+++ b/attendance-sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Documents/trainings/general/react/react-itc-may-14-31-2018/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89375018-FB85-6C45-8EF6-E393C0FB5931}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51869584-0DA1-0E4A-8D23-32EF807E323B}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14660" xr2:uid="{CBB9C8E6-5B3B-8049-96F8-54CD5DF45308}"/>
   </bookViews>
@@ -477,7 +477,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="15" fontId="1" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -493,6 +492,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
@@ -1283,8 +1283,8 @@
   <dimension ref="A1:R26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="P24" sqref="P24"/>
+      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1337,7 +1337,7 @@
       <c r="L1" s="13">
         <v>43245</v>
       </c>
-      <c r="M1" s="25">
+      <c r="M1" s="24">
         <v>43246</v>
       </c>
       <c r="N1" s="13">
@@ -1385,7 +1385,7 @@
       <c r="L2" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="M2" s="26" t="s">
+      <c r="M2" s="25" t="s">
         <v>42</v>
       </c>
       <c r="N2" s="15" t="s">
@@ -1418,8 +1418,8 @@
       <c r="G3" s="17"/>
       <c r="H3" s="17"/>
       <c r="I3" s="17"/>
-      <c r="J3" s="31"/>
-      <c r="K3" s="31"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="30"/>
       <c r="L3" s="17"/>
       <c r="M3" s="17"/>
       <c r="N3" s="17"/>
@@ -1444,13 +1444,13 @@
       <c r="H4" s="17"/>
       <c r="I4" s="17"/>
       <c r="J4" s="17"/>
-      <c r="K4" s="31"/>
+      <c r="K4" s="30"/>
       <c r="L4" s="17"/>
       <c r="M4" s="17"/>
       <c r="N4" s="17"/>
       <c r="O4" s="17"/>
       <c r="P4" s="17"/>
-      <c r="Q4" s="20"/>
+      <c r="Q4" s="17"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
@@ -1462,20 +1462,20 @@
       <c r="C5" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="31"/>
-      <c r="K5" s="31"/>
-      <c r="L5" s="20"/>
-      <c r="M5" s="27"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="30"/>
+      <c r="K5" s="30"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="26"/>
       <c r="N5" s="17"/>
       <c r="O5" s="17"/>
       <c r="P5" s="17"/>
-      <c r="Q5" s="20"/>
+      <c r="Q5" s="17"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
@@ -1492,15 +1492,15 @@
       <c r="F6" s="17"/>
       <c r="G6" s="17"/>
       <c r="H6" s="17"/>
-      <c r="I6" s="31"/>
-      <c r="J6" s="31"/>
-      <c r="K6" s="31"/>
-      <c r="L6" s="31"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="30"/>
+      <c r="K6" s="30"/>
+      <c r="L6" s="30"/>
       <c r="M6" s="17"/>
-      <c r="N6" s="20"/>
+      <c r="N6" s="19"/>
       <c r="O6" s="17"/>
       <c r="P6" s="17"/>
-      <c r="Q6" s="20"/>
+      <c r="Q6" s="17"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
@@ -1518,14 +1518,14 @@
       <c r="G7" s="18"/>
       <c r="H7" s="18"/>
       <c r="I7" s="17"/>
-      <c r="J7" s="31"/>
+      <c r="J7" s="30"/>
       <c r="K7" s="17"/>
-      <c r="L7" s="31"/>
+      <c r="L7" s="30"/>
       <c r="M7" s="17"/>
       <c r="N7" s="17"/>
       <c r="O7" s="17"/>
       <c r="P7" s="17"/>
-      <c r="Q7" s="20"/>
+      <c r="Q7" s="17"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
@@ -1542,15 +1542,15 @@
       <c r="F8" s="17"/>
       <c r="G8" s="17"/>
       <c r="H8" s="17"/>
-      <c r="I8" s="31"/>
-      <c r="J8" s="31"/>
+      <c r="I8" s="30"/>
+      <c r="J8" s="30"/>
       <c r="K8" s="17"/>
       <c r="L8" s="17"/>
       <c r="M8" s="17"/>
       <c r="N8" s="17"/>
       <c r="O8" s="17"/>
       <c r="P8" s="17"/>
-      <c r="Q8" s="20"/>
+      <c r="Q8" s="17"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
@@ -1563,19 +1563,19 @@
         <v>16</v>
       </c>
       <c r="D9" s="18"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
       <c r="G9" s="18"/>
       <c r="H9" s="18"/>
-      <c r="I9" s="32"/>
-      <c r="J9" s="32"/>
-      <c r="K9" s="32"/>
-      <c r="L9" s="32"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="31"/>
+      <c r="L9" s="31"/>
       <c r="M9" s="17"/>
       <c r="N9" s="17"/>
       <c r="O9" s="17"/>
       <c r="P9" s="17"/>
-      <c r="Q9" s="20"/>
+      <c r="Q9" s="17"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
@@ -1587,20 +1587,20 @@
       <c r="C10" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="32"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="20"/>
-      <c r="M10" s="27"/>
-      <c r="N10" s="20"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="19"/>
+      <c r="M10" s="26"/>
+      <c r="N10" s="19"/>
       <c r="O10" s="17"/>
       <c r="P10" s="17"/>
-      <c r="Q10" s="20"/>
+      <c r="Q10" s="17"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
@@ -1617,15 +1617,15 @@
       <c r="F11" s="17"/>
       <c r="G11" s="17"/>
       <c r="H11" s="17"/>
-      <c r="I11" s="31"/>
-      <c r="J11" s="31"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="30"/>
       <c r="K11" s="17"/>
       <c r="L11" s="17"/>
-      <c r="M11" s="27"/>
+      <c r="M11" s="26"/>
       <c r="N11" s="17"/>
       <c r="O11" s="17"/>
-      <c r="P11" s="20"/>
-      <c r="Q11" s="20"/>
+      <c r="P11" s="19"/>
+      <c r="Q11" s="17"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
@@ -1638,19 +1638,19 @@
         <v>22</v>
       </c>
       <c r="D12" s="17"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="23"/>
-      <c r="I12" s="23"/>
-      <c r="J12" s="31"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="30"/>
       <c r="K12" s="17"/>
-      <c r="L12" s="20"/>
+      <c r="L12" s="19"/>
       <c r="M12" s="17"/>
       <c r="N12" s="17"/>
       <c r="O12" s="17"/>
-      <c r="P12" s="20"/>
-      <c r="Q12" s="20"/>
+      <c r="P12" s="19"/>
+      <c r="Q12" s="17"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
@@ -1663,19 +1663,19 @@
         <v>24</v>
       </c>
       <c r="D13" s="17"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
       <c r="G13" s="18"/>
       <c r="H13" s="18"/>
-      <c r="I13" s="23"/>
-      <c r="J13" s="20"/>
-      <c r="K13" s="20"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="19"/>
       <c r="L13" s="17"/>
-      <c r="M13" s="27"/>
+      <c r="M13" s="26"/>
       <c r="N13" s="17"/>
       <c r="O13" s="17"/>
       <c r="P13" s="17"/>
-      <c r="Q13" s="20"/>
+      <c r="Q13" s="32"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
@@ -1692,15 +1692,15 @@
       <c r="F14" s="18"/>
       <c r="G14" s="18"/>
       <c r="H14" s="18"/>
-      <c r="I14" s="20"/>
-      <c r="J14" s="20"/>
-      <c r="K14" s="20"/>
-      <c r="L14" s="20"/>
-      <c r="M14" s="27"/>
-      <c r="N14" s="20"/>
-      <c r="O14" s="20"/>
-      <c r="P14" s="20"/>
-      <c r="Q14" s="20"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="19"/>
+      <c r="K14" s="19"/>
+      <c r="L14" s="19"/>
+      <c r="M14" s="26"/>
+      <c r="N14" s="19"/>
+      <c r="O14" s="19"/>
+      <c r="P14" s="19"/>
+      <c r="Q14" s="32"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
@@ -1718,14 +1718,14 @@
       <c r="G15" s="17"/>
       <c r="H15" s="17"/>
       <c r="I15" s="17"/>
-      <c r="J15" s="31"/>
-      <c r="K15" s="31"/>
-      <c r="L15" s="31"/>
+      <c r="J15" s="30"/>
+      <c r="K15" s="30"/>
+      <c r="L15" s="30"/>
       <c r="M15" s="17"/>
-      <c r="N15" s="20"/>
+      <c r="N15" s="19"/>
       <c r="O15" s="17"/>
       <c r="P15" s="17"/>
-      <c r="Q15" s="20"/>
+      <c r="Q15" s="17"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
@@ -1738,19 +1738,19 @@
         <v>30</v>
       </c>
       <c r="D16" s="17"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="23"/>
-      <c r="I16" s="23"/>
-      <c r="J16" s="31"/>
-      <c r="K16" s="31"/>
-      <c r="L16" s="31"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="30"/>
+      <c r="K16" s="30"/>
+      <c r="L16" s="30"/>
       <c r="M16" s="17"/>
       <c r="N16" s="17"/>
       <c r="O16" s="17"/>
       <c r="P16" s="17"/>
-      <c r="Q16" s="20"/>
+      <c r="Q16" s="17"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
@@ -1769,13 +1769,13 @@
       <c r="H17" s="17"/>
       <c r="I17" s="17"/>
       <c r="J17" s="17"/>
-      <c r="K17" s="31"/>
+      <c r="K17" s="30"/>
       <c r="L17" s="17"/>
       <c r="M17" s="17"/>
       <c r="N17" s="17"/>
       <c r="O17" s="17"/>
       <c r="P17" s="17"/>
-      <c r="Q17" s="20"/>
+      <c r="Q17" s="17"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
@@ -1783,20 +1783,20 @@
       </c>
       <c r="B18" s="9"/>
       <c r="C18" s="10"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="21"/>
-      <c r="I18" s="21"/>
-      <c r="J18" s="21"/>
-      <c r="K18" s="21"/>
-      <c r="L18" s="21"/>
-      <c r="M18" s="29"/>
-      <c r="N18" s="21"/>
-      <c r="O18" s="21"/>
-      <c r="P18" s="21"/>
-      <c r="Q18" s="21"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="20"/>
+      <c r="L18" s="20"/>
+      <c r="M18" s="28"/>
+      <c r="N18" s="20"/>
+      <c r="O18" s="20"/>
+      <c r="P18" s="20"/>
+      <c r="Q18" s="32"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
@@ -1809,19 +1809,19 @@
         <v>51</v>
       </c>
       <c r="D19" s="18"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="23"/>
-      <c r="G19" s="23"/>
-      <c r="H19" s="23"/>
-      <c r="I19" s="31"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="30"/>
       <c r="J19" s="17"/>
       <c r="K19" s="17"/>
-      <c r="L19" s="21"/>
+      <c r="L19" s="20"/>
       <c r="M19" s="17"/>
       <c r="N19" s="17"/>
       <c r="O19" s="17"/>
-      <c r="P19" s="21"/>
-      <c r="Q19" s="21"/>
+      <c r="P19" s="20"/>
+      <c r="Q19" s="17"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
@@ -1838,15 +1838,15 @@
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
       <c r="H20" s="17"/>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="30"/>
       <c r="K20" s="17"/>
-      <c r="L20" s="31"/>
+      <c r="L20" s="30"/>
       <c r="M20" s="17"/>
-      <c r="N20" s="20"/>
-      <c r="O20" s="20"/>
+      <c r="N20" s="19"/>
+      <c r="O20" s="19"/>
       <c r="P20" s="17"/>
-      <c r="Q20" s="20"/>
+      <c r="Q20" s="17"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
@@ -1864,14 +1864,14 @@
       <c r="G21" s="17"/>
       <c r="H21" s="17"/>
       <c r="I21" s="17"/>
-      <c r="J21" s="31"/>
+      <c r="J21" s="30"/>
       <c r="K21" s="17"/>
       <c r="L21" s="17"/>
-      <c r="M21" s="27"/>
+      <c r="M21" s="26"/>
       <c r="N21" s="17"/>
       <c r="O21" s="17"/>
       <c r="P21" s="17"/>
-      <c r="Q21" s="20"/>
+      <c r="Q21" s="17"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
@@ -1889,35 +1889,35 @@
       <c r="G22" s="17"/>
       <c r="H22" s="17"/>
       <c r="I22" s="17"/>
-      <c r="J22" s="31"/>
+      <c r="J22" s="30"/>
       <c r="K22" s="17"/>
       <c r="L22" s="17"/>
       <c r="M22" s="17"/>
       <c r="N22" s="17"/>
       <c r="O22" s="17"/>
       <c r="P22" s="17"/>
-      <c r="Q22" s="20"/>
+      <c r="Q22" s="17"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A23" s="30" t="s">
+      <c r="A23" s="29" t="s">
         <v>52</v>
       </c>
       <c r="B23" s="9"/>
       <c r="C23" s="10"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="23"/>
-      <c r="G23" s="23"/>
-      <c r="H23" s="23"/>
-      <c r="I23" s="23"/>
-      <c r="J23" s="31"/>
-      <c r="K23" s="31"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="22"/>
+      <c r="J23" s="30"/>
+      <c r="K23" s="30"/>
       <c r="L23" s="17"/>
       <c r="M23" s="17"/>
       <c r="N23" s="17"/>
       <c r="O23" s="17"/>
       <c r="P23" s="17"/>
-      <c r="Q23" s="18"/>
+      <c r="Q23" s="17"/>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
@@ -1929,20 +1929,20 @@
       <c r="C24" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="D24" s="23"/>
-      <c r="E24" s="23"/>
-      <c r="F24" s="23"/>
-      <c r="G24" s="23"/>
-      <c r="H24" s="23"/>
-      <c r="I24" s="23"/>
-      <c r="J24" s="31"/>
-      <c r="K24" s="22"/>
-      <c r="L24" s="22"/>
-      <c r="M24" s="28"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="22"/>
+      <c r="I24" s="22"/>
+      <c r="J24" s="30"/>
+      <c r="K24" s="21"/>
+      <c r="L24" s="21"/>
+      <c r="M24" s="27"/>
       <c r="N24" s="17"/>
       <c r="O24" s="17"/>
       <c r="P24" s="17"/>
-      <c r="Q24" s="22"/>
+      <c r="Q24" s="17"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="G26" s="11"/>

</xml_diff>